<commit_message>
updated conifer master sheet beofre the collection day
</commit_message>
<xml_diff>
--- a/data_sheets2019/collection_broadlvs.xlsx
+++ b/data_sheets2019/collection_broadlvs.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">collection_broadlvs.csv!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="18">
   <si>
     <t>species</t>
   </si>
@@ -71,12 +71,18 @@
   <si>
     <t>UMCA</t>
   </si>
+  <si>
+    <t>only one near kerris hous</t>
+  </si>
+  <si>
+    <t>down the road</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -101,6 +107,24 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -119,14 +143,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -458,29 +488,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F321"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="5.1640625" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="3"/>
     <col min="5" max="5" width="22.6640625" customWidth="1"/>
     <col min="6" max="6" width="37.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="20" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -490,263 +521,551 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="20" customHeight="1">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="C2" s="3">
+        <v>606006</v>
+      </c>
+      <c r="D2" s="3">
+        <v>4023900</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="20" customHeight="1">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="C3" s="3">
+        <v>606007</v>
+      </c>
+      <c r="D3" s="3">
+        <v>4023900</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="20" customHeight="1">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="C4" s="3">
+        <v>606011</v>
+      </c>
+      <c r="D4" s="3">
+        <v>4023894</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="20" customHeight="1">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="C5" s="3">
+        <v>606026</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4023890</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="20" customHeight="1">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="C6" s="3">
+        <v>606032</v>
+      </c>
+      <c r="D6" s="3">
+        <v>4023879</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="20" customHeight="1">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="C7" s="3">
+        <v>606032</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4023879</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="20" customHeight="1">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="C8" s="3">
+        <v>606144</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4023903</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="20" customHeight="1">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="C9" s="3">
+        <v>606162</v>
+      </c>
+      <c r="D9" s="3">
+        <v>4023899</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="20" customHeight="1">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="C10" s="3">
+        <v>606173</v>
+      </c>
+      <c r="D10" s="3">
+        <v>4023908</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="20" customHeight="1">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="C11" s="3">
+        <v>606190</v>
+      </c>
+      <c r="D11" s="3">
+        <v>4023915</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="20" customHeight="1">
       <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="C12" s="3">
+        <v>606190</v>
+      </c>
+      <c r="D12" s="3">
+        <v>4023915</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="20" customHeight="1">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="C13" s="3">
+        <v>606256</v>
+      </c>
+      <c r="D13" s="3">
+        <v>4023936</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="20" customHeight="1">
       <c r="A14" t="s">
         <v>6</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="C14" s="3">
+        <v>606291</v>
+      </c>
+      <c r="D14" s="3">
+        <v>4023923</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="20" customHeight="1">
       <c r="A15" t="s">
         <v>6</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="C15" s="3">
+        <v>606324</v>
+      </c>
+      <c r="D15" s="3">
+        <v>4023880</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="20" customHeight="1">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" s="3">
+        <v>606335</v>
+      </c>
+      <c r="D16" s="3">
+        <v>4023948</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="20" customHeight="1">
       <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" s="3">
+        <v>606330</v>
+      </c>
+      <c r="D17" s="3">
+        <v>4023945</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="20" customHeight="1">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" s="3">
+        <v>606330</v>
+      </c>
+      <c r="D18" s="3">
+        <v>4023945</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="20" customHeight="1">
       <c r="A19" t="s">
         <v>6</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" s="3">
+        <v>606306</v>
+      </c>
+      <c r="D19" s="3">
+        <v>4023954</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="20" customHeight="1">
       <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" s="3">
+        <v>606302</v>
+      </c>
+      <c r="D20" s="3">
+        <v>4023964</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="20" customHeight="1">
       <c r="A21" t="s">
         <v>6</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" s="3">
+        <v>606291</v>
+      </c>
+      <c r="D21" s="3">
+        <v>4023962</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="20" customHeight="1">
       <c r="A22" t="s">
         <v>6</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" s="3">
+        <v>606291</v>
+      </c>
+      <c r="D22" s="3">
+        <v>4023962</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="20" customHeight="1">
       <c r="A23" t="s">
         <v>6</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" s="3">
+        <v>606291</v>
+      </c>
+      <c r="D23" s="3">
+        <v>4023962</v>
+      </c>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="20" customHeight="1">
       <c r="A24" t="s">
         <v>6</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" s="3">
+        <v>606291</v>
+      </c>
+      <c r="D24" s="3">
+        <v>4023962</v>
+      </c>
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="20" customHeight="1">
       <c r="A25" t="s">
         <v>6</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" s="3">
+        <v>606292</v>
+      </c>
+      <c r="D25" s="3">
+        <v>4023969</v>
+      </c>
+      <c r="E25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="20" customHeight="1">
       <c r="A26" t="s">
         <v>6</v>
       </c>
       <c r="B26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" s="3">
+        <v>606288</v>
+      </c>
+      <c r="D26" s="3">
+        <v>4023968</v>
+      </c>
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="20" customHeight="1">
       <c r="A27" t="s">
         <v>6</v>
       </c>
       <c r="B27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" s="3">
+        <v>606281</v>
+      </c>
+      <c r="D27" s="3">
+        <v>4023962</v>
+      </c>
+      <c r="E27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="20" customHeight="1">
       <c r="A28" t="s">
         <v>6</v>
       </c>
       <c r="B28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" s="3">
+        <v>606219</v>
+      </c>
+      <c r="D28" s="3">
+        <v>4024020</v>
+      </c>
+      <c r="E28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="20" customHeight="1">
       <c r="A29" t="s">
         <v>6</v>
       </c>
       <c r="B29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" s="3">
+        <v>606219</v>
+      </c>
+      <c r="D29" s="3">
+        <v>4024020</v>
+      </c>
+      <c r="E29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="20" customHeight="1">
       <c r="A30" t="s">
         <v>6</v>
       </c>
       <c r="B30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" s="3">
+        <v>606219</v>
+      </c>
+      <c r="D30" s="3">
+        <v>4024020</v>
+      </c>
+      <c r="E30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="20" customHeight="1">
       <c r="A31" t="s">
         <v>6</v>
       </c>
       <c r="B31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" s="3">
+        <v>606281</v>
+      </c>
+      <c r="D31" s="3">
+        <v>4023983</v>
+      </c>
+      <c r="E31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="20" customHeight="1">
       <c r="A32" t="s">
         <v>6</v>
       </c>
       <c r="B32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" s="3">
+        <v>606256</v>
+      </c>
+      <c r="D32" s="3">
+        <v>4023973</v>
+      </c>
+      <c r="E32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="20" customHeight="1">
       <c r="A33" t="s">
         <v>6</v>
       </c>
       <c r="B33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" s="3">
+        <v>606026</v>
+      </c>
+      <c r="D33" s="3">
+        <v>4023761</v>
+      </c>
+      <c r="E33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="20" customHeight="1">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -754,7 +1073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:5" ht="20" customHeight="1">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -762,7 +1081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:5" ht="20" customHeight="1">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -770,7 +1089,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:5" ht="20" customHeight="1">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -778,7 +1097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:5" ht="20" customHeight="1">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -786,7 +1105,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:5" ht="20" customHeight="1">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -794,7 +1113,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:5" ht="20" customHeight="1">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -802,7 +1121,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:5" ht="20" customHeight="1">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -810,7 +1129,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:5" ht="20" customHeight="1">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -818,7 +1137,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:5" ht="20" customHeight="1">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -826,7 +1145,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:5" ht="20" customHeight="1">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -834,7 +1153,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:5" ht="20" customHeight="1">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -842,7 +1161,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:5" ht="20" customHeight="1">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -850,7 +1169,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:5" ht="20" customHeight="1">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -858,7 +1177,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:5" ht="20" customHeight="1">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -866,7 +1185,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" ht="20" customHeight="1">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -874,7 +1193,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" ht="20" customHeight="1">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -882,7 +1201,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" ht="20" customHeight="1">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -890,7 +1209,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" ht="20" customHeight="1">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -898,7 +1217,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" ht="20" customHeight="1">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -906,7 +1225,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" ht="20" customHeight="1">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -914,7 +1233,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" ht="20" customHeight="1">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -922,7 +1241,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" ht="20" customHeight="1">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -930,7 +1249,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" ht="20" customHeight="1">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -938,7 +1257,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" ht="20" customHeight="1">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -946,7 +1265,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" ht="20" customHeight="1">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -954,7 +1273,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" ht="20" customHeight="1">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -962,7 +1281,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" ht="20" customHeight="1">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -970,7 +1289,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" ht="20" customHeight="1">
       <c r="A62" t="s">
         <v>7</v>
       </c>
@@ -978,7 +1297,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" ht="20" customHeight="1">
       <c r="A63" t="s">
         <v>7</v>
       </c>
@@ -986,7 +1305,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" ht="20" customHeight="1">
       <c r="A64" t="s">
         <v>7</v>
       </c>
@@ -994,7 +1313,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" ht="20" customHeight="1">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -1002,7 +1321,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" ht="20" customHeight="1">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -1010,7 +1329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" ht="20" customHeight="1">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -1018,7 +1337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" ht="20" customHeight="1">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -1026,7 +1345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" ht="20" customHeight="1">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -1034,7 +1353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" ht="20" customHeight="1">
       <c r="A70" t="s">
         <v>8</v>
       </c>
@@ -1042,7 +1361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" ht="20" customHeight="1">
       <c r="A71" t="s">
         <v>8</v>
       </c>
@@ -1050,7 +1369,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" ht="20" customHeight="1">
       <c r="A72" t="s">
         <v>8</v>
       </c>
@@ -1058,7 +1377,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" ht="20" customHeight="1">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -1066,7 +1385,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" ht="20" customHeight="1">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -1074,7 +1393,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" ht="20" customHeight="1">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -1082,7 +1401,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" ht="20" customHeight="1">
       <c r="A76" t="s">
         <v>8</v>
       </c>
@@ -1090,7 +1409,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" ht="20" customHeight="1">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -1098,7 +1417,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" ht="20" customHeight="1">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -1106,7 +1425,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" ht="20" customHeight="1">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -1114,7 +1433,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" ht="20" customHeight="1">
       <c r="A80" t="s">
         <v>8</v>
       </c>
@@ -1122,7 +1441,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" ht="20" customHeight="1">
       <c r="A81" t="s">
         <v>8</v>
       </c>
@@ -1130,7 +1449,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" ht="20" customHeight="1">
       <c r="A82" t="s">
         <v>8</v>
       </c>
@@ -1138,7 +1457,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" ht="20" customHeight="1">
       <c r="A83" t="s">
         <v>8</v>
       </c>
@@ -1146,7 +1465,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" ht="20" customHeight="1">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -1154,7 +1473,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" ht="20" customHeight="1">
       <c r="A85" t="s">
         <v>8</v>
       </c>
@@ -1162,7 +1481,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" ht="20" customHeight="1">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -1170,7 +1489,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" ht="20" customHeight="1">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -1178,7 +1497,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" ht="20" customHeight="1">
       <c r="A88" t="s">
         <v>8</v>
       </c>
@@ -1186,7 +1505,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" ht="20" customHeight="1">
       <c r="A89" t="s">
         <v>8</v>
       </c>
@@ -1194,7 +1513,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" ht="20" customHeight="1">
       <c r="A90" t="s">
         <v>8</v>
       </c>
@@ -1202,7 +1521,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" ht="20" customHeight="1">
       <c r="A91" t="s">
         <v>8</v>
       </c>
@@ -1210,7 +1529,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" ht="20" customHeight="1">
       <c r="A92" t="s">
         <v>8</v>
       </c>
@@ -1218,7 +1537,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" ht="20" customHeight="1">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -1226,7 +1545,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" ht="20" customHeight="1">
       <c r="A94" t="s">
         <v>8</v>
       </c>
@@ -1234,7 +1553,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" ht="20" customHeight="1">
       <c r="A95" t="s">
         <v>8</v>
       </c>
@@ -1242,7 +1561,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" ht="20" customHeight="1">
       <c r="A96" t="s">
         <v>8</v>
       </c>
@@ -1250,7 +1569,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" ht="20" customHeight="1">
       <c r="A97" t="s">
         <v>8</v>
       </c>
@@ -1258,7 +1577,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" ht="20" customHeight="1">
       <c r="A98" t="s">
         <v>9</v>
       </c>
@@ -1266,7 +1585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" ht="20" customHeight="1">
       <c r="A99" t="s">
         <v>9</v>
       </c>
@@ -1274,7 +1593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" ht="20" customHeight="1">
       <c r="A100" t="s">
         <v>9</v>
       </c>
@@ -1282,7 +1601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" ht="20" customHeight="1">
       <c r="A101" t="s">
         <v>9</v>
       </c>
@@ -1290,7 +1609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" ht="20" customHeight="1">
       <c r="A102" t="s">
         <v>9</v>
       </c>
@@ -1298,7 +1617,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" ht="20" customHeight="1">
       <c r="A103" t="s">
         <v>9</v>
       </c>
@@ -1306,7 +1625,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" ht="20" customHeight="1">
       <c r="A104" t="s">
         <v>9</v>
       </c>
@@ -1314,7 +1633,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" ht="20" customHeight="1">
       <c r="A105" t="s">
         <v>9</v>
       </c>
@@ -1322,7 +1641,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" ht="20" customHeight="1">
       <c r="A106" t="s">
         <v>9</v>
       </c>
@@ -1330,7 +1649,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" ht="20" customHeight="1">
       <c r="A107" t="s">
         <v>9</v>
       </c>
@@ -1338,7 +1657,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" ht="20" customHeight="1">
       <c r="A108" t="s">
         <v>9</v>
       </c>
@@ -1346,7 +1665,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" ht="20" customHeight="1">
       <c r="A109" t="s">
         <v>9</v>
       </c>
@@ -1354,7 +1673,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" ht="20" customHeight="1">
       <c r="A110" t="s">
         <v>9</v>
       </c>
@@ -1362,7 +1681,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" ht="20" customHeight="1">
       <c r="A111" t="s">
         <v>9</v>
       </c>
@@ -1370,7 +1689,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" ht="20" customHeight="1">
       <c r="A112" t="s">
         <v>9</v>
       </c>
@@ -1378,7 +1697,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" ht="20" customHeight="1">
       <c r="A113" t="s">
         <v>9</v>
       </c>
@@ -1386,7 +1705,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" ht="20" customHeight="1">
       <c r="A114" t="s">
         <v>9</v>
       </c>
@@ -1394,7 +1713,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" ht="20" customHeight="1">
       <c r="A115" t="s">
         <v>9</v>
       </c>
@@ -1402,7 +1721,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" ht="20" customHeight="1">
       <c r="A116" t="s">
         <v>9</v>
       </c>
@@ -1410,7 +1729,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" ht="20" customHeight="1">
       <c r="A117" t="s">
         <v>9</v>
       </c>
@@ -1418,7 +1737,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" ht="20" customHeight="1">
       <c r="A118" t="s">
         <v>9</v>
       </c>
@@ -1426,7 +1745,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" ht="20" customHeight="1">
       <c r="A119" t="s">
         <v>9</v>
       </c>
@@ -1434,7 +1753,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" ht="20" customHeight="1">
       <c r="A120" t="s">
         <v>9</v>
       </c>
@@ -1442,7 +1761,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" ht="20" customHeight="1">
       <c r="A121" t="s">
         <v>9</v>
       </c>
@@ -1450,7 +1769,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" ht="20" customHeight="1">
       <c r="A122" t="s">
         <v>9</v>
       </c>
@@ -1458,7 +1777,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" ht="20" customHeight="1">
       <c r="A123" t="s">
         <v>9</v>
       </c>
@@ -1466,7 +1785,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" ht="20" customHeight="1">
       <c r="A124" t="s">
         <v>9</v>
       </c>
@@ -1474,7 +1793,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" ht="20" customHeight="1">
       <c r="A125" t="s">
         <v>9</v>
       </c>
@@ -1482,7 +1801,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" ht="20" customHeight="1">
       <c r="A126" t="s">
         <v>9</v>
       </c>
@@ -1490,7 +1809,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" ht="20" customHeight="1">
       <c r="A127" t="s">
         <v>9</v>
       </c>
@@ -1498,7 +1817,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" ht="20" customHeight="1">
       <c r="A128" t="s">
         <v>9</v>
       </c>
@@ -1506,7 +1825,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" ht="20" customHeight="1">
       <c r="A129" t="s">
         <v>9</v>
       </c>
@@ -1514,7 +1833,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" ht="20" customHeight="1">
       <c r="A130" t="s">
         <v>10</v>
       </c>
@@ -1522,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" ht="20" customHeight="1">
       <c r="A131" t="s">
         <v>10</v>
       </c>
@@ -1530,7 +1849,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" ht="20" customHeight="1">
       <c r="A132" t="s">
         <v>10</v>
       </c>
@@ -1538,7 +1857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" ht="20" customHeight="1">
       <c r="A133" t="s">
         <v>10</v>
       </c>
@@ -1546,7 +1865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" ht="20" customHeight="1">
       <c r="A134" t="s">
         <v>10</v>
       </c>
@@ -1554,7 +1873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" ht="20" customHeight="1">
       <c r="A135" t="s">
         <v>10</v>
       </c>
@@ -1562,7 +1881,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" ht="20" customHeight="1">
       <c r="A136" t="s">
         <v>10</v>
       </c>
@@ -1570,7 +1889,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" ht="20" customHeight="1">
       <c r="A137" t="s">
         <v>10</v>
       </c>
@@ -1578,7 +1897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" ht="20" customHeight="1">
       <c r="A138" t="s">
         <v>10</v>
       </c>
@@ -1586,7 +1905,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" ht="20" customHeight="1">
       <c r="A139" t="s">
         <v>10</v>
       </c>
@@ -1594,7 +1913,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" ht="20" customHeight="1">
       <c r="A140" t="s">
         <v>10</v>
       </c>
@@ -1602,7 +1921,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" ht="20" customHeight="1">
       <c r="A141" t="s">
         <v>10</v>
       </c>
@@ -1610,7 +1929,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" ht="20" customHeight="1">
       <c r="A142" t="s">
         <v>10</v>
       </c>
@@ -1618,7 +1937,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" ht="20" customHeight="1">
       <c r="A143" t="s">
         <v>10</v>
       </c>
@@ -1626,7 +1945,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" ht="20" customHeight="1">
       <c r="A144" t="s">
         <v>10</v>
       </c>
@@ -1634,7 +1953,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" ht="20" customHeight="1">
       <c r="A145" t="s">
         <v>10</v>
       </c>
@@ -1642,7 +1961,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" ht="20" customHeight="1">
       <c r="A146" t="s">
         <v>10</v>
       </c>
@@ -1650,7 +1969,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" ht="20" customHeight="1">
       <c r="A147" t="s">
         <v>10</v>
       </c>
@@ -1658,7 +1977,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" ht="20" customHeight="1">
       <c r="A148" t="s">
         <v>10</v>
       </c>
@@ -1666,7 +1985,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" ht="20" customHeight="1">
       <c r="A149" t="s">
         <v>10</v>
       </c>
@@ -1674,7 +1993,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" ht="20" customHeight="1">
       <c r="A150" t="s">
         <v>10</v>
       </c>
@@ -1682,7 +2001,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" ht="20" customHeight="1">
       <c r="A151" t="s">
         <v>10</v>
       </c>
@@ -1690,7 +2009,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" ht="20" customHeight="1">
       <c r="A152" t="s">
         <v>10</v>
       </c>
@@ -1698,7 +2017,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" ht="20" customHeight="1">
       <c r="A153" t="s">
         <v>10</v>
       </c>
@@ -1706,7 +2025,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" ht="20" customHeight="1">
       <c r="A154" t="s">
         <v>10</v>
       </c>
@@ -1714,7 +2033,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" ht="20" customHeight="1">
       <c r="A155" t="s">
         <v>10</v>
       </c>
@@ -1722,7 +2041,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" ht="20" customHeight="1">
       <c r="A156" t="s">
         <v>10</v>
       </c>
@@ -1730,7 +2049,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" ht="20" customHeight="1">
       <c r="A157" t="s">
         <v>10</v>
       </c>
@@ -1738,7 +2057,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" ht="20" customHeight="1">
       <c r="A158" t="s">
         <v>10</v>
       </c>
@@ -1746,7 +2065,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" ht="20" customHeight="1">
       <c r="A159" t="s">
         <v>10</v>
       </c>
@@ -1754,7 +2073,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" ht="20" customHeight="1">
       <c r="A160" t="s">
         <v>10</v>
       </c>
@@ -1762,7 +2081,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" ht="20" customHeight="1">
       <c r="A161" t="s">
         <v>10</v>
       </c>
@@ -1770,7 +2089,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" ht="20" customHeight="1">
       <c r="A162" t="s">
         <v>11</v>
       </c>
@@ -1778,7 +2097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" ht="20" customHeight="1">
       <c r="A163" t="s">
         <v>11</v>
       </c>
@@ -1786,7 +2105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" ht="20" customHeight="1">
       <c r="A164" t="s">
         <v>11</v>
       </c>
@@ -1794,7 +2113,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" ht="20" customHeight="1">
       <c r="A165" t="s">
         <v>11</v>
       </c>
@@ -1802,7 +2121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" ht="20" customHeight="1">
       <c r="A166" t="s">
         <v>11</v>
       </c>
@@ -1810,7 +2129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" ht="20" customHeight="1">
       <c r="A167" t="s">
         <v>11</v>
       </c>
@@ -1818,7 +2137,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" ht="20" customHeight="1">
       <c r="A168" t="s">
         <v>11</v>
       </c>
@@ -1826,7 +2145,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" ht="20" customHeight="1">
       <c r="A169" t="s">
         <v>11</v>
       </c>
@@ -1834,7 +2153,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" ht="20" customHeight="1">
       <c r="A170" t="s">
         <v>11</v>
       </c>
@@ -1842,7 +2161,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" ht="20" customHeight="1">
       <c r="A171" t="s">
         <v>11</v>
       </c>
@@ -1850,7 +2169,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" ht="20" customHeight="1">
       <c r="A172" t="s">
         <v>11</v>
       </c>
@@ -1858,7 +2177,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" ht="20" customHeight="1">
       <c r="A173" t="s">
         <v>11</v>
       </c>
@@ -1866,7 +2185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" ht="20" customHeight="1">
       <c r="A174" t="s">
         <v>11</v>
       </c>
@@ -1874,7 +2193,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" ht="20" customHeight="1">
       <c r="A175" t="s">
         <v>11</v>
       </c>
@@ -1882,7 +2201,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" ht="20" customHeight="1">
       <c r="A176" t="s">
         <v>11</v>
       </c>
@@ -1890,7 +2209,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" ht="20" customHeight="1">
       <c r="A177" t="s">
         <v>11</v>
       </c>
@@ -1898,7 +2217,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" ht="20" customHeight="1">
       <c r="A178" t="s">
         <v>11</v>
       </c>
@@ -1906,7 +2225,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" ht="20" customHeight="1">
       <c r="A179" t="s">
         <v>11</v>
       </c>
@@ -1914,7 +2233,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" ht="20" customHeight="1">
       <c r="A180" t="s">
         <v>11</v>
       </c>
@@ -1922,7 +2241,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" ht="20" customHeight="1">
       <c r="A181" t="s">
         <v>11</v>
       </c>
@@ -1930,7 +2249,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" ht="20" customHeight="1">
       <c r="A182" t="s">
         <v>11</v>
       </c>
@@ -1938,7 +2257,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" ht="20" customHeight="1">
       <c r="A183" t="s">
         <v>11</v>
       </c>
@@ -1946,7 +2265,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" ht="20" customHeight="1">
       <c r="A184" t="s">
         <v>11</v>
       </c>
@@ -1954,7 +2273,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" ht="20" customHeight="1">
       <c r="A185" t="s">
         <v>11</v>
       </c>
@@ -1962,7 +2281,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" ht="20" customHeight="1">
       <c r="A186" t="s">
         <v>11</v>
       </c>
@@ -1970,7 +2289,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" ht="20" customHeight="1">
       <c r="A187" t="s">
         <v>11</v>
       </c>
@@ -1978,7 +2297,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" ht="20" customHeight="1">
       <c r="A188" t="s">
         <v>11</v>
       </c>
@@ -1986,7 +2305,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" ht="20" customHeight="1">
       <c r="A189" t="s">
         <v>11</v>
       </c>
@@ -1994,7 +2313,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" ht="20" customHeight="1">
       <c r="A190" t="s">
         <v>11</v>
       </c>
@@ -2002,7 +2321,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" ht="20" customHeight="1">
       <c r="A191" t="s">
         <v>11</v>
       </c>
@@ -2010,7 +2329,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" ht="20" customHeight="1">
       <c r="A192" t="s">
         <v>11</v>
       </c>
@@ -2018,7 +2337,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" ht="20" customHeight="1">
       <c r="A193" t="s">
         <v>11</v>
       </c>
@@ -2026,7 +2345,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" ht="20" customHeight="1">
       <c r="A194" t="s">
         <v>12</v>
       </c>
@@ -2034,7 +2353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" ht="20" customHeight="1">
       <c r="A195" t="s">
         <v>12</v>
       </c>
@@ -2042,7 +2361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" ht="20" customHeight="1">
       <c r="A196" t="s">
         <v>12</v>
       </c>
@@ -2050,7 +2369,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" ht="20" customHeight="1">
       <c r="A197" t="s">
         <v>12</v>
       </c>
@@ -2058,7 +2377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:2">
+    <row r="198" spans="1:2" ht="20" customHeight="1">
       <c r="A198" t="s">
         <v>12</v>
       </c>
@@ -2066,7 +2385,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" ht="20" customHeight="1">
       <c r="A199" t="s">
         <v>12</v>
       </c>
@@ -2074,7 +2393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" ht="20" customHeight="1">
       <c r="A200" t="s">
         <v>12</v>
       </c>
@@ -2082,7 +2401,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" ht="20" customHeight="1">
       <c r="A201" t="s">
         <v>12</v>
       </c>
@@ -2090,7 +2409,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" ht="20" customHeight="1">
       <c r="A202" t="s">
         <v>12</v>
       </c>
@@ -2098,7 +2417,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" ht="20" customHeight="1">
       <c r="A203" t="s">
         <v>12</v>
       </c>
@@ -2106,7 +2425,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" ht="20" customHeight="1">
       <c r="A204" t="s">
         <v>12</v>
       </c>
@@ -2114,7 +2433,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" ht="20" customHeight="1">
       <c r="A205" t="s">
         <v>12</v>
       </c>
@@ -2122,7 +2441,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" ht="20" customHeight="1">
       <c r="A206" t="s">
         <v>12</v>
       </c>
@@ -2130,7 +2449,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" ht="20" customHeight="1">
       <c r="A207" t="s">
         <v>12</v>
       </c>
@@ -2138,7 +2457,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" ht="20" customHeight="1">
       <c r="A208" t="s">
         <v>12</v>
       </c>
@@ -2146,7 +2465,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" ht="20" customHeight="1">
       <c r="A209" t="s">
         <v>12</v>
       </c>
@@ -2154,7 +2473,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" ht="20" customHeight="1">
       <c r="A210" t="s">
         <v>12</v>
       </c>
@@ -2162,7 +2481,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" ht="20" customHeight="1">
       <c r="A211" t="s">
         <v>12</v>
       </c>
@@ -2170,7 +2489,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" ht="20" customHeight="1">
       <c r="A212" t="s">
         <v>12</v>
       </c>
@@ -2178,7 +2497,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="213" spans="1:2">
+    <row r="213" spans="1:2" ht="20" customHeight="1">
       <c r="A213" t="s">
         <v>12</v>
       </c>
@@ -2186,7 +2505,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" ht="20" customHeight="1">
       <c r="A214" t="s">
         <v>12</v>
       </c>
@@ -2194,7 +2513,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="215" spans="1:2">
+    <row r="215" spans="1:2" ht="20" customHeight="1">
       <c r="A215" t="s">
         <v>12</v>
       </c>
@@ -2202,7 +2521,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="216" spans="1:2">
+    <row r="216" spans="1:2" ht="20" customHeight="1">
       <c r="A216" t="s">
         <v>12</v>
       </c>
@@ -2210,7 +2529,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="217" spans="1:2">
+    <row r="217" spans="1:2" ht="20" customHeight="1">
       <c r="A217" t="s">
         <v>12</v>
       </c>
@@ -2218,7 +2537,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="218" spans="1:2">
+    <row r="218" spans="1:2" ht="20" customHeight="1">
       <c r="A218" t="s">
         <v>12</v>
       </c>
@@ -2226,7 +2545,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="219" spans="1:2">
+    <row r="219" spans="1:2" ht="20" customHeight="1">
       <c r="A219" t="s">
         <v>12</v>
       </c>
@@ -2234,7 +2553,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="220" spans="1:2">
+    <row r="220" spans="1:2" ht="20" customHeight="1">
       <c r="A220" t="s">
         <v>12</v>
       </c>
@@ -2242,7 +2561,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:2">
+    <row r="221" spans="1:2" ht="20" customHeight="1">
       <c r="A221" t="s">
         <v>12</v>
       </c>
@@ -2250,7 +2569,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:2">
+    <row r="222" spans="1:2" ht="20" customHeight="1">
       <c r="A222" t="s">
         <v>12</v>
       </c>
@@ -2258,7 +2577,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="223" spans="1:2">
+    <row r="223" spans="1:2" ht="20" customHeight="1">
       <c r="A223" t="s">
         <v>12</v>
       </c>
@@ -2266,7 +2585,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="224" spans="1:2">
+    <row r="224" spans="1:2" ht="20" customHeight="1">
       <c r="A224" t="s">
         <v>12</v>
       </c>
@@ -2274,7 +2593,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" ht="20" customHeight="1">
       <c r="A225" t="s">
         <v>12</v>
       </c>
@@ -2282,7 +2601,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" ht="20" customHeight="1">
       <c r="A226" t="s">
         <v>13</v>
       </c>
@@ -2290,7 +2609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" ht="20" customHeight="1">
       <c r="A227" t="s">
         <v>13</v>
       </c>
@@ -2298,7 +2617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="1:2">
+    <row r="228" spans="1:2" ht="20" customHeight="1">
       <c r="A228" t="s">
         <v>13</v>
       </c>
@@ -2306,7 +2625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="229" spans="1:2">
+    <row r="229" spans="1:2" ht="20" customHeight="1">
       <c r="A229" t="s">
         <v>13</v>
       </c>
@@ -2314,7 +2633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="230" spans="1:2">
+    <row r="230" spans="1:2" ht="20" customHeight="1">
       <c r="A230" t="s">
         <v>13</v>
       </c>
@@ -2322,7 +2641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="1:2">
+    <row r="231" spans="1:2" ht="20" customHeight="1">
       <c r="A231" t="s">
         <v>13</v>
       </c>
@@ -2330,7 +2649,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="232" spans="1:2">
+    <row r="232" spans="1:2" ht="20" customHeight="1">
       <c r="A232" t="s">
         <v>13</v>
       </c>
@@ -2338,7 +2657,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="233" spans="1:2">
+    <row r="233" spans="1:2" ht="20" customHeight="1">
       <c r="A233" t="s">
         <v>13</v>
       </c>
@@ -2346,7 +2665,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="234" spans="1:2">
+    <row r="234" spans="1:2" ht="20" customHeight="1">
       <c r="A234" t="s">
         <v>13</v>
       </c>
@@ -2354,7 +2673,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="235" spans="1:2">
+    <row r="235" spans="1:2" ht="20" customHeight="1">
       <c r="A235" t="s">
         <v>13</v>
       </c>
@@ -2362,7 +2681,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="236" spans="1:2">
+    <row r="236" spans="1:2" ht="20" customHeight="1">
       <c r="A236" t="s">
         <v>13</v>
       </c>
@@ -2370,7 +2689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:2">
+    <row r="237" spans="1:2" ht="20" customHeight="1">
       <c r="A237" t="s">
         <v>13</v>
       </c>
@@ -2378,7 +2697,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:2" ht="20" customHeight="1">
       <c r="A238" t="s">
         <v>13</v>
       </c>
@@ -2386,7 +2705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="239" spans="1:2">
+    <row r="239" spans="1:2" ht="20" customHeight="1">
       <c r="A239" t="s">
         <v>13</v>
       </c>
@@ -2394,7 +2713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="240" spans="1:2">
+    <row r="240" spans="1:2" ht="20" customHeight="1">
       <c r="A240" t="s">
         <v>13</v>
       </c>
@@ -2402,7 +2721,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:2" ht="20" customHeight="1">
       <c r="A241" t="s">
         <v>13</v>
       </c>
@@ -2410,7 +2729,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="242" spans="1:2">
+    <row r="242" spans="1:2" ht="20" customHeight="1">
       <c r="A242" t="s">
         <v>13</v>
       </c>
@@ -2418,7 +2737,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="243" spans="1:2">
+    <row r="243" spans="1:2" ht="20" customHeight="1">
       <c r="A243" t="s">
         <v>13</v>
       </c>
@@ -2426,7 +2745,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="244" spans="1:2">
+    <row r="244" spans="1:2" ht="20" customHeight="1">
       <c r="A244" t="s">
         <v>13</v>
       </c>
@@ -2434,7 +2753,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="245" spans="1:2">
+    <row r="245" spans="1:2" ht="20" customHeight="1">
       <c r="A245" t="s">
         <v>13</v>
       </c>
@@ -2442,7 +2761,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="246" spans="1:2">
+    <row r="246" spans="1:2" ht="20" customHeight="1">
       <c r="A246" t="s">
         <v>13</v>
       </c>
@@ -2450,7 +2769,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="247" spans="1:2">
+    <row r="247" spans="1:2" ht="20" customHeight="1">
       <c r="A247" t="s">
         <v>13</v>
       </c>
@@ -2458,7 +2777,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="248" spans="1:2">
+    <row r="248" spans="1:2" ht="20" customHeight="1">
       <c r="A248" t="s">
         <v>13</v>
       </c>
@@ -2466,7 +2785,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="249" spans="1:2">
+    <row r="249" spans="1:2" ht="20" customHeight="1">
       <c r="A249" t="s">
         <v>13</v>
       </c>
@@ -2474,7 +2793,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="250" spans="1:2">
+    <row r="250" spans="1:2" ht="20" customHeight="1">
       <c r="A250" t="s">
         <v>13</v>
       </c>
@@ -2482,7 +2801,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="251" spans="1:2">
+    <row r="251" spans="1:2" ht="20" customHeight="1">
       <c r="A251" t="s">
         <v>13</v>
       </c>
@@ -2490,7 +2809,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="252" spans="1:2">
+    <row r="252" spans="1:2" ht="20" customHeight="1">
       <c r="A252" t="s">
         <v>13</v>
       </c>
@@ -2498,7 +2817,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="253" spans="1:2">
+    <row r="253" spans="1:2" ht="20" customHeight="1">
       <c r="A253" t="s">
         <v>13</v>
       </c>
@@ -2506,7 +2825,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="254" spans="1:2">
+    <row r="254" spans="1:2" ht="20" customHeight="1">
       <c r="A254" t="s">
         <v>13</v>
       </c>
@@ -2514,7 +2833,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="255" spans="1:2">
+    <row r="255" spans="1:2" ht="20" customHeight="1">
       <c r="A255" t="s">
         <v>13</v>
       </c>
@@ -2522,7 +2841,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="256" spans="1:2">
+    <row r="256" spans="1:2" ht="20" customHeight="1">
       <c r="A256" t="s">
         <v>13</v>
       </c>
@@ -2530,7 +2849,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="257" spans="1:2">
+    <row r="257" spans="1:2" ht="20" customHeight="1">
       <c r="A257" t="s">
         <v>13</v>
       </c>
@@ -2538,7 +2857,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="258" spans="1:2">
+    <row r="258" spans="1:2" ht="20" customHeight="1">
       <c r="A258" t="s">
         <v>14</v>
       </c>
@@ -2546,7 +2865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:2">
+    <row r="259" spans="1:2" ht="20" customHeight="1">
       <c r="A259" t="s">
         <v>14</v>
       </c>
@@ -2554,7 +2873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="260" spans="1:2">
+    <row r="260" spans="1:2" ht="20" customHeight="1">
       <c r="A260" t="s">
         <v>14</v>
       </c>
@@ -2562,7 +2881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="261" spans="1:2">
+    <row r="261" spans="1:2" ht="20" customHeight="1">
       <c r="A261" t="s">
         <v>14</v>
       </c>
@@ -2570,7 +2889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="262" spans="1:2">
+    <row r="262" spans="1:2" ht="20" customHeight="1">
       <c r="A262" t="s">
         <v>14</v>
       </c>
@@ -2578,7 +2897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="263" spans="1:2">
+    <row r="263" spans="1:2" ht="20" customHeight="1">
       <c r="A263" t="s">
         <v>14</v>
       </c>
@@ -2586,7 +2905,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="264" spans="1:2">
+    <row r="264" spans="1:2" ht="20" customHeight="1">
       <c r="A264" t="s">
         <v>14</v>
       </c>
@@ -2594,7 +2913,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="265" spans="1:2">
+    <row r="265" spans="1:2" ht="20" customHeight="1">
       <c r="A265" t="s">
         <v>14</v>
       </c>
@@ -2602,7 +2921,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="266" spans="1:2">
+    <row r="266" spans="1:2" ht="20" customHeight="1">
       <c r="A266" t="s">
         <v>14</v>
       </c>
@@ -2610,7 +2929,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="267" spans="1:2">
+    <row r="267" spans="1:2" ht="20" customHeight="1">
       <c r="A267" t="s">
         <v>14</v>
       </c>
@@ -2618,7 +2937,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="268" spans="1:2">
+    <row r="268" spans="1:2" ht="20" customHeight="1">
       <c r="A268" t="s">
         <v>14</v>
       </c>
@@ -2626,7 +2945,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="269" spans="1:2">
+    <row r="269" spans="1:2" ht="20" customHeight="1">
       <c r="A269" t="s">
         <v>14</v>
       </c>
@@ -2634,7 +2953,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="270" spans="1:2">
+    <row r="270" spans="1:2" ht="20" customHeight="1">
       <c r="A270" t="s">
         <v>14</v>
       </c>
@@ -2642,7 +2961,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="271" spans="1:2">
+    <row r="271" spans="1:2" ht="20" customHeight="1">
       <c r="A271" t="s">
         <v>14</v>
       </c>
@@ -2650,7 +2969,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="272" spans="1:2">
+    <row r="272" spans="1:2" ht="20" customHeight="1">
       <c r="A272" t="s">
         <v>14</v>
       </c>
@@ -2658,7 +2977,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="273" spans="1:2">
+    <row r="273" spans="1:2" ht="20" customHeight="1">
       <c r="A273" t="s">
         <v>14</v>
       </c>
@@ -2666,7 +2985,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="274" spans="1:2">
+    <row r="274" spans="1:2" ht="20" customHeight="1">
       <c r="A274" t="s">
         <v>14</v>
       </c>
@@ -2674,7 +2993,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="275" spans="1:2">
+    <row r="275" spans="1:2" ht="20" customHeight="1">
       <c r="A275" t="s">
         <v>14</v>
       </c>
@@ -2682,7 +3001,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="276" spans="1:2">
+    <row r="276" spans="1:2" ht="20" customHeight="1">
       <c r="A276" t="s">
         <v>14</v>
       </c>
@@ -2690,7 +3009,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="277" spans="1:2">
+    <row r="277" spans="1:2" ht="20" customHeight="1">
       <c r="A277" t="s">
         <v>14</v>
       </c>
@@ -2698,7 +3017,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="278" spans="1:2">
+    <row r="278" spans="1:2" ht="20" customHeight="1">
       <c r="A278" t="s">
         <v>14</v>
       </c>
@@ -2706,7 +3025,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="279" spans="1:2">
+    <row r="279" spans="1:2" ht="20" customHeight="1">
       <c r="A279" t="s">
         <v>14</v>
       </c>
@@ -2714,7 +3033,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="280" spans="1:2">
+    <row r="280" spans="1:2" ht="20" customHeight="1">
       <c r="A280" t="s">
         <v>14</v>
       </c>
@@ -2722,7 +3041,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="281" spans="1:2">
+    <row r="281" spans="1:2" ht="20" customHeight="1">
       <c r="A281" t="s">
         <v>14</v>
       </c>
@@ -2730,7 +3049,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="282" spans="1:2">
+    <row r="282" spans="1:2" ht="20" customHeight="1">
       <c r="A282" t="s">
         <v>14</v>
       </c>
@@ -2738,7 +3057,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="283" spans="1:2">
+    <row r="283" spans="1:2" ht="20" customHeight="1">
       <c r="A283" t="s">
         <v>14</v>
       </c>
@@ -2746,7 +3065,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="284" spans="1:2">
+    <row r="284" spans="1:2" ht="20" customHeight="1">
       <c r="A284" t="s">
         <v>14</v>
       </c>
@@ -2754,7 +3073,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="285" spans="1:2">
+    <row r="285" spans="1:2" ht="20" customHeight="1">
       <c r="A285" t="s">
         <v>14</v>
       </c>
@@ -2762,7 +3081,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="286" spans="1:2">
+    <row r="286" spans="1:2" ht="20" customHeight="1">
       <c r="A286" t="s">
         <v>14</v>
       </c>
@@ -2770,7 +3089,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="287" spans="1:2">
+    <row r="287" spans="1:2" ht="20" customHeight="1">
       <c r="A287" t="s">
         <v>14</v>
       </c>
@@ -2778,7 +3097,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="288" spans="1:2">
+    <row r="288" spans="1:2" ht="20" customHeight="1">
       <c r="A288" t="s">
         <v>14</v>
       </c>
@@ -2786,7 +3105,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="289" spans="1:2">
+    <row r="289" spans="1:2" ht="20" customHeight="1">
       <c r="A289" t="s">
         <v>14</v>
       </c>
@@ -2794,7 +3113,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="290" spans="1:2">
+    <row r="290" spans="1:2" ht="20" customHeight="1">
       <c r="A290" t="s">
         <v>15</v>
       </c>
@@ -2802,7 +3121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:2">
+    <row r="291" spans="1:2" ht="20" customHeight="1">
       <c r="A291" t="s">
         <v>15</v>
       </c>
@@ -2810,7 +3129,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="292" spans="1:2">
+    <row r="292" spans="1:2" ht="20" customHeight="1">
       <c r="A292" t="s">
         <v>15</v>
       </c>
@@ -2818,7 +3137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="293" spans="1:2">
+    <row r="293" spans="1:2" ht="20" customHeight="1">
       <c r="A293" t="s">
         <v>15</v>
       </c>
@@ -2826,7 +3145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="294" spans="1:2">
+    <row r="294" spans="1:2" ht="20" customHeight="1">
       <c r="A294" t="s">
         <v>15</v>
       </c>
@@ -2834,7 +3153,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="295" spans="1:2">
+    <row r="295" spans="1:2" ht="20" customHeight="1">
       <c r="A295" t="s">
         <v>15</v>
       </c>
@@ -2842,7 +3161,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="296" spans="1:2">
+    <row r="296" spans="1:2" ht="20" customHeight="1">
       <c r="A296" t="s">
         <v>15</v>
       </c>
@@ -2850,7 +3169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="297" spans="1:2">
+    <row r="297" spans="1:2" ht="20" customHeight="1">
       <c r="A297" t="s">
         <v>15</v>
       </c>
@@ -2858,7 +3177,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="298" spans="1:2">
+    <row r="298" spans="1:2" ht="20" customHeight="1">
       <c r="A298" t="s">
         <v>15</v>
       </c>
@@ -2866,7 +3185,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="299" spans="1:2">
+    <row r="299" spans="1:2" ht="20" customHeight="1">
       <c r="A299" t="s">
         <v>15</v>
       </c>
@@ -2874,7 +3193,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="300" spans="1:2">
+    <row r="300" spans="1:2" ht="20" customHeight="1">
       <c r="A300" t="s">
         <v>15</v>
       </c>
@@ -2882,7 +3201,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="301" spans="1:2">
+    <row r="301" spans="1:2" ht="20" customHeight="1">
       <c r="A301" t="s">
         <v>15</v>
       </c>
@@ -2890,7 +3209,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="302" spans="1:2">
+    <row r="302" spans="1:2" ht="20" customHeight="1">
       <c r="A302" t="s">
         <v>15</v>
       </c>
@@ -2898,7 +3217,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="303" spans="1:2">
+    <row r="303" spans="1:2" ht="20" customHeight="1">
       <c r="A303" t="s">
         <v>15</v>
       </c>
@@ -2906,7 +3225,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="304" spans="1:2">
+    <row r="304" spans="1:2" ht="20" customHeight="1">
       <c r="A304" t="s">
         <v>15</v>
       </c>
@@ -2914,7 +3233,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="305" spans="1:2">
+    <row r="305" spans="1:2" ht="20" customHeight="1">
       <c r="A305" t="s">
         <v>15</v>
       </c>
@@ -2922,7 +3241,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="306" spans="1:2">
+    <row r="306" spans="1:2" ht="20" customHeight="1">
       <c r="A306" t="s">
         <v>15</v>
       </c>
@@ -2930,7 +3249,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="307" spans="1:2">
+    <row r="307" spans="1:2" ht="20" customHeight="1">
       <c r="A307" t="s">
         <v>15</v>
       </c>
@@ -2938,7 +3257,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="308" spans="1:2">
+    <row r="308" spans="1:2" ht="20" customHeight="1">
       <c r="A308" t="s">
         <v>15</v>
       </c>
@@ -2946,7 +3265,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="309" spans="1:2">
+    <row r="309" spans="1:2" ht="20" customHeight="1">
       <c r="A309" t="s">
         <v>15</v>
       </c>
@@ -2954,7 +3273,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="310" spans="1:2">
+    <row r="310" spans="1:2" ht="20" customHeight="1">
       <c r="A310" t="s">
         <v>15</v>
       </c>
@@ -2962,7 +3281,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="311" spans="1:2">
+    <row r="311" spans="1:2" ht="20" customHeight="1">
       <c r="A311" t="s">
         <v>15</v>
       </c>
@@ -2970,7 +3289,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="312" spans="1:2">
+    <row r="312" spans="1:2" ht="20" customHeight="1">
       <c r="A312" t="s">
         <v>15</v>
       </c>
@@ -2978,7 +3297,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="313" spans="1:2">
+    <row r="313" spans="1:2" ht="20" customHeight="1">
       <c r="A313" t="s">
         <v>15</v>
       </c>
@@ -2986,7 +3305,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="314" spans="1:2">
+    <row r="314" spans="1:2" ht="20" customHeight="1">
       <c r="A314" t="s">
         <v>15</v>
       </c>
@@ -2994,7 +3313,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="315" spans="1:2">
+    <row r="315" spans="1:2" ht="20" customHeight="1">
       <c r="A315" t="s">
         <v>15</v>
       </c>
@@ -3002,7 +3321,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="316" spans="1:2">
+    <row r="316" spans="1:2" ht="20" customHeight="1">
       <c r="A316" t="s">
         <v>15</v>
       </c>
@@ -3010,7 +3329,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="317" spans="1:2">
+    <row r="317" spans="1:2" ht="20" customHeight="1">
       <c r="A317" t="s">
         <v>15</v>
       </c>
@@ -3018,7 +3337,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="318" spans="1:2">
+    <row r="318" spans="1:2" ht="20" customHeight="1">
       <c r="A318" t="s">
         <v>15</v>
       </c>
@@ -3026,7 +3345,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="319" spans="1:2">
+    <row r="319" spans="1:2" ht="20" customHeight="1">
       <c r="A319" t="s">
         <v>15</v>
       </c>
@@ -3034,7 +3353,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="320" spans="1:2">
+    <row r="320" spans="1:2" ht="20" customHeight="1">
       <c r="A320" t="s">
         <v>15</v>
       </c>
@@ -3042,7 +3361,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="321" spans="1:2">
+    <row r="321" spans="1:2" ht="20" customHeight="1">
       <c r="A321" t="s">
         <v>15</v>
       </c>
@@ -3052,14 +3371,15 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.72222222222222221" header="0.3" footer="0.25"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;LCollectors: _______________________x000D_Date: 5/11/19&amp;C&amp;"-,Bold"Competency Project: _x000D_Broad-leafed species&amp;"-,Regular"_x000D_&amp;RPage &amp;P_x000D__x000D_</oddHeader>
   </headerFooter>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>